<commit_message>
änderung doku und entscheidungstabelle
</commit_message>
<xml_diff>
--- a/12_Entscheidungstabelle (1).xlsx
+++ b/12_Entscheidungstabelle (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\Schule\IMS\Informatik\Modul 431\projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57B861-3710-414B-8802-A43CC03C9ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C683CFA-89F2-4E8E-88F5-995D0A179510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Entscheidungstabelle</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Teilnutzwert</t>
   </si>
   <si>
-    <t>Variante 1</t>
-  </si>
-  <si>
     <t>Beschreibung der Gewichtungen:</t>
   </si>
   <si>
@@ -285,13 +282,13 @@
     <t>Gesamtnutzwert</t>
   </si>
   <si>
-    <t>Variante 2</t>
-  </si>
-  <si>
     <t>Mittels einer groben Aufwand/Kosten-Abschätzung kann vorausgesagt werden, wie lange es benötigt, die Variante umzusetzen. Die Gewichtung wurde auf hohe 25% gelegt, da verbesserte Usability, Performance, Gestaltung und Security meist in höherem Aufwand resultiert. [...]</t>
   </si>
   <si>
-    <t>Variante X</t>
+    <t>Wireframe Florian</t>
+  </si>
+  <si>
+    <t>Wireframe Noel</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -567,7 +564,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -869,7 +865,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -886,20 +882,18 @@
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="32"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="53" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
@@ -921,62 +915,60 @@
       <c r="H3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>10</v>
-      </c>
+      <c r="I3" s="13"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="19">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D4" s="22">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" s="23">
         <f>C$4*D4</f>
-        <v>0.6</v>
+        <v>1.75</v>
       </c>
       <c r="F4" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <f>C$4*F4</f>
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="20">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D5" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E5" s="17">
-        <f t="shared" ref="E5:E9" si="0">C$4*D5</f>
-        <v>2.4</v>
+        <f>C$5*D5</f>
+        <v>0.75</v>
       </c>
       <c r="F5" s="11">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G5" s="10">
-        <f t="shared" ref="G5:G9" si="1">C$4*F5</f>
-        <v>0.6</v>
+        <f>C$5*F5</f>
+        <v>1.05</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="17"/>
@@ -986,51 +978,51 @@
       <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
+      <c r="A6" s="30"/>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="19">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D6" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E6" s="15">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
+        <f>C$6*D6</f>
+        <v>2.8</v>
       </c>
       <c r="F6" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>C$6*F6</f>
+        <v>2.4499999999999997</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="16">
-        <v>7</v>
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
       </c>
       <c r="E7" s="17">
-        <f t="shared" si="0"/>
-        <v>2.1</v>
+        <f>C$7*D7</f>
+        <v>0.05</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
       </c>
       <c r="G7" s="10">
-        <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <f>C$7*F7</f>
+        <v>0.15000000000000002</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
@@ -1040,51 +1032,51 @@
       <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
+      <c r="A8" s="30"/>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="19">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D8" s="14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8" s="15">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999998</v>
+        <f>C$8*D8</f>
+        <v>0.6</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <f>C$8*F8</f>
+        <v>1.3499999999999999</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="31"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="20">
         <v>0.05</v>
       </c>
-      <c r="D9" s="26">
-        <v>4</v>
-      </c>
-      <c r="E9" s="27">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
+      <c r="D9" s="14">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <f>C$9*D9</f>
+        <v>0.4</v>
       </c>
       <c r="F9" s="11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" si="1"/>
-        <v>2.6999999999999997</v>
+        <f>C$9*F9</f>
+        <v>0.35000000000000003</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="17"/>
@@ -1097,7 +1089,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="21">
         <f>SUM(C4:C9)</f>
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
@@ -1112,7 +1104,7 @@
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="24" t="str">
@@ -1121,17 +1113,17 @@
       </c>
       <c r="E11" s="25">
         <f>SUM(E4:E9)</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="F11" s="29" t="str">
+        <v>6.35</v>
+      </c>
+      <c r="F11" s="28" t="str">
         <f>"1."</f>
         <v>1.</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <f>SUM(G4:G9)</f>
-        <v>10.5</v>
-      </c>
-      <c r="H11" s="28"/>
+        <v>6.85</v>
+      </c>
+      <c r="H11" s="27"/>
       <c r="I11" s="25"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -1141,21 +1133,21 @@
     <row r="12" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
+      <c r="B14" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>